<commit_message>
Validate required if other field value in list
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/required_values.xlsx
+++ b/openn/tests/data/sheets/required_values.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>Note: Please enter one work per page.</t>
   </si>
@@ -176,15 +176,52 @@
   </si>
   <si>
     <t>Field 6 (not required, value)</t>
+  </si>
+  <si>
+    <t>Field 7</t>
+  </si>
+  <si>
+    <t>Field 9 (repeating)</t>
+  </si>
+  <si>
+    <t>Required if 7 is CAT (valid)</t>
+  </si>
+  <si>
+    <t>Required if 7 is CAT (invalid)</t>
+  </si>
+  <si>
+    <t>Require if field 8 is CAT (valid)</t>
+  </si>
+  <si>
+    <t>Required if 9 is CAT</t>
+  </si>
+  <si>
+    <t>Field 8 (cat is lower case)</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>DOG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -280,93 +317,110 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="15" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -404,6 +458,14 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -430,6 +492,14 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="15"/>
   </cellStyles>
@@ -730,13 +800,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -957,16 +1027,75 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>